<commit_message>
update Luban.Server to latest version
</commit_message>
<xml_diff>
--- a/DesignerConfigs/Datas/test/test_null.xlsx
+++ b/DesignerConfigs/Datas/test/test_null.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\luban_examples\DesignerConfigs\Datas\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA411CB0-6135-43B7-8799-62FB813AC746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE53C091-171B-4B43-B971-D79EDE4D4387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E1D40A03-67D6-4B72-8D32-2FA0B71CC234}"/>
+    <workbookView xWindow="1140" yWindow="1155" windowWidth="27645" windowHeight="14865" xr2:uid="{E1D40A03-67D6-4B72-8D32-2FA0B71CC234}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>##</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -48,10 +48,6 @@
   </si>
   <si>
     <t>null</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>{null}</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -475,7 +471,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -500,7 +496,7 @@
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -516,10 +512,10 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -530,16 +526,16 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6">
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H6">
         <v>1</v>

</xml_diff>